<commit_message>
fuck det her projekt
</commit_message>
<xml_diff>
--- a/project/Gantt-chart.xlsx
+++ b/project/Gantt-chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ny Bruger\Desktop\optilogic-project\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39EFAA7-F670-4A69-9262-BA81752EAA1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01AB5B11-CCBB-443B-8E88-61693277234F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="645" yWindow="1275" windowWidth="24990" windowHeight="12615" xr2:uid="{99CF4FEF-5634-4449-A34D-5735707B8B12}"/>
+    <workbookView xWindow="1275" yWindow="525" windowWidth="26655" windowHeight="14430" xr2:uid="{99CF4FEF-5634-4449-A34D-5735707B8B12}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
-  <si>
-    <t>Gantt chart</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>ID</t>
   </si>
@@ -98,9 +95,6 @@
     <t>November</t>
   </si>
   <si>
-    <t>December</t>
-  </si>
-  <si>
     <t>Projektafgrænsning</t>
   </si>
   <si>
@@ -143,19 +137,7 @@
     <t>MQTT User</t>
   </si>
   <si>
-    <t>15.</t>
-  </si>
-  <si>
-    <t>16.</t>
-  </si>
-  <si>
-    <t>17.</t>
-  </si>
-  <si>
-    <t>18.</t>
-  </si>
-  <si>
-    <t>19.</t>
+    <t>Gantt chart OptiLogic</t>
   </si>
 </sst>
 </file>
@@ -216,7 +198,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -329,11 +311,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -343,15 +365,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -361,25 +384,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -718,8 +764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E237C772-8E61-4360-B74C-AFD62B3AE3E1}">
   <dimension ref="A1:T27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,60 +774,108 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
+      <c r="A1" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
     </row>
     <row r="2" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="31"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+    </row>
+    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="32"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="33"/>
+      <c r="R3" s="24"/>
+      <c r="S3" s="24"/>
+      <c r="T3" s="24"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="15"/>
+      <c r="D4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="21" t="s">
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="21" t="s">
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="R4" s="14"/>
-      <c r="S4" s="14"/>
-      <c r="T4" s="15"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="18"/>
+      <c r="S4" s="18"/>
+      <c r="T4" s="18"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="21"/>
       <c r="D5" s="6">
         <v>36</v>
       </c>
@@ -818,30 +912,24 @@
       <c r="O5" s="6">
         <v>47</v>
       </c>
-      <c r="P5" s="6">
+      <c r="P5" s="22">
         <v>48</v>
       </c>
-      <c r="Q5" s="6">
+      <c r="Q5" s="5">
         <v>49</v>
       </c>
-      <c r="R5" s="6">
-        <v>50</v>
-      </c>
-      <c r="S5" s="6">
-        <v>51</v>
-      </c>
-      <c r="T5" s="6">
-        <v>52</v>
-      </c>
+      <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
+      <c r="T5" s="16"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="20"/>
+      <c r="A6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="15"/>
       <c r="D6" s="2"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -854,20 +942,20 @@
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
+      <c r="P6" s="10"/>
       <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="5"/>
-      <c r="T6" s="5"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="18"/>
+      <c r="A7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="15"/>
       <c r="D7" s="2"/>
       <c r="E7" s="3"/>
       <c r="F7" s="5"/>
@@ -880,25 +968,25 @@
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
+      <c r="P7" s="10"/>
       <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
-      <c r="T7" s="5"/>
+      <c r="R7" s="16"/>
+      <c r="S7" s="16"/>
+      <c r="T7" s="16"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="11"/>
+      <c r="A8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="15"/>
+      <c r="D8" s="9"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="10"/>
+      <c r="H8" s="8"/>
       <c r="I8" s="5"/>
       <c r="J8" s="4"/>
       <c r="K8" s="5"/>
@@ -906,21 +994,21 @@
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
+      <c r="P8" s="10"/>
       <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5"/>
+      <c r="R8" s="16"/>
+      <c r="S8" s="16"/>
+      <c r="T8" s="16"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="11"/>
+      <c r="A9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="15"/>
+      <c r="D9" s="9"/>
       <c r="E9" s="3"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
@@ -932,21 +1020,21 @@
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
+      <c r="P9" s="10"/>
       <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="16"/>
+      <c r="T9" s="16"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="11"/>
+      <c r="A10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="15"/>
+      <c r="D10" s="9"/>
       <c r="E10" s="3"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
@@ -958,99 +1046,99 @@
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
+      <c r="P10" s="10"/>
       <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
+      <c r="R10" s="16"/>
+      <c r="S10" s="16"/>
+      <c r="T10" s="16"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="11"/>
+      <c r="A11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="15"/>
+      <c r="D11" s="9"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="5"/>
+      <c r="I11" s="3"/>
       <c r="J11" s="4"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
+      <c r="P11" s="10"/>
       <c r="Q11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
-      <c r="T11" s="5"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="16"/>
+      <c r="T11" s="16"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="11"/>
+      <c r="A12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="15"/>
+      <c r="D12" s="9"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="5"/>
+      <c r="I12" s="3"/>
       <c r="J12" s="4"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
+      <c r="P12" s="10"/>
       <c r="Q12" s="5"/>
-      <c r="R12" s="5"/>
-      <c r="S12" s="5"/>
-      <c r="T12" s="5"/>
+      <c r="R12" s="16"/>
+      <c r="S12" s="16"/>
+      <c r="T12" s="16"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="11"/>
+      <c r="A13" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="15"/>
+      <c r="D13" s="9"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="4"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="5"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="3"/>
       <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
+      <c r="P13" s="10"/>
       <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="5"/>
-      <c r="T13" s="5"/>
+      <c r="R13" s="16"/>
+      <c r="S13" s="16"/>
+      <c r="T13" s="16"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="11"/>
+      <c r="A14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="15"/>
+      <c r="D14" s="9"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -1059,50 +1147,50 @@
       <c r="J14" s="4"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
-      <c r="M14" s="10"/>
+      <c r="M14" s="8"/>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
+      <c r="P14" s="10"/>
       <c r="Q14" s="5"/>
-      <c r="R14" s="5"/>
-      <c r="S14" s="5"/>
-      <c r="T14" s="5"/>
+      <c r="R14" s="16"/>
+      <c r="S14" s="16"/>
+      <c r="T14" s="16"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="11"/>
+      <c r="A15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="15"/>
+      <c r="D15" s="9"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="3"/>
       <c r="J15" s="4"/>
-      <c r="K15" s="5"/>
+      <c r="K15" s="3"/>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
-      <c r="P15" s="5"/>
+      <c r="P15" s="10"/>
       <c r="Q15" s="5"/>
-      <c r="R15" s="5"/>
-      <c r="S15" s="5"/>
-      <c r="T15" s="5"/>
+      <c r="R15" s="16"/>
+      <c r="S15" s="16"/>
+      <c r="T15" s="16"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="11"/>
+      <c r="A16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="15"/>
+      <c r="D16" s="9"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="3"/>
@@ -1114,21 +1202,21 @@
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
+      <c r="P16" s="10"/>
       <c r="Q16" s="5"/>
-      <c r="R16" s="5"/>
-      <c r="S16" s="5"/>
-      <c r="T16" s="5"/>
+      <c r="R16" s="16"/>
+      <c r="S16" s="16"/>
+      <c r="T16" s="16"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="11"/>
+      <c r="A17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="9"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
@@ -1140,47 +1228,47 @@
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="5"/>
-      <c r="T17" s="5"/>
+      <c r="P17" s="23"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="16"/>
+      <c r="S17" s="16"/>
+      <c r="T17" s="16"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="11"/>
+      <c r="A18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="9"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="I18" s="3"/>
       <c r="J18" s="4"/>
-      <c r="K18" s="5"/>
+      <c r="K18" s="3"/>
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
+      <c r="P18" s="10"/>
       <c r="Q18" s="5"/>
-      <c r="R18" s="5"/>
-      <c r="S18" s="5"/>
-      <c r="T18" s="5"/>
+      <c r="R18" s="16"/>
+      <c r="S18" s="16"/>
+      <c r="T18" s="16"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="11"/>
+      <c r="A19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="9"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
@@ -1192,131 +1280,121 @@
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
+      <c r="P19" s="10"/>
       <c r="Q19" s="5"/>
-      <c r="R19" s="5"/>
-      <c r="S19" s="5"/>
-      <c r="T19" s="5"/>
+      <c r="R19" s="16"/>
+      <c r="S19" s="16"/>
+      <c r="T19" s="16"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
-      <c r="P20" s="5"/>
-      <c r="Q20" s="5"/>
-      <c r="R20" s="5"/>
-      <c r="S20" s="5"/>
-      <c r="T20" s="5"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="16"/>
+      <c r="R20" s="16"/>
+      <c r="S20" s="16"/>
+      <c r="T20" s="16"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="5"/>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="5"/>
-      <c r="R21" s="5"/>
-      <c r="S21" s="5"/>
-      <c r="T21" s="5"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="16"/>
+      <c r="P21" s="16"/>
+      <c r="Q21" s="16"/>
+      <c r="R21" s="16"/>
+      <c r="S21" s="16"/>
+      <c r="T21" s="16"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="5"/>
-      <c r="P22" s="5"/>
-      <c r="Q22" s="5"/>
-      <c r="R22" s="5"/>
-      <c r="S22" s="5"/>
-      <c r="T22" s="5"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="16"/>
+      <c r="P22" s="16"/>
+      <c r="Q22" s="16"/>
+      <c r="R22" s="16"/>
+      <c r="S22" s="16"/>
+      <c r="T22" s="16"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" s="14"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
-      <c r="O23" s="5"/>
-      <c r="P23" s="5"/>
-      <c r="Q23" s="5"/>
-      <c r="R23" s="5"/>
-      <c r="S23" s="5"/>
-      <c r="T23" s="5"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="16"/>
+      <c r="Q23" s="16"/>
+      <c r="R23" s="16"/>
+      <c r="S23" s="16"/>
+      <c r="T23" s="16"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="14"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
-      <c r="O24" s="5"/>
-      <c r="P24" s="5"/>
-      <c r="Q24" s="5"/>
-      <c r="R24" s="5"/>
-      <c r="S24" s="5"/>
-      <c r="T24" s="5"/>
+      <c r="A24" s="16"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="16"/>
+      <c r="O24" s="16"/>
+      <c r="P24" s="16"/>
+      <c r="Q24" s="16"/>
+      <c r="R24" s="16"/>
+      <c r="S24" s="16"/>
+      <c r="T24" s="16"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
@@ -1331,23 +1409,8 @@
       <c r="D27" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="A1:C3"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="H4:L4"/>
-    <mergeCell ref="M4:P4"/>
-    <mergeCell ref="Q4:T4"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
+  <mergeCells count="20">
     <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B21:C21"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
@@ -1357,8 +1420,19 @@
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="M4:P4"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="H4:L4"/>
+    <mergeCell ref="A1:Q3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>